<commit_message>
minor tweaks to openxml template's headers
</commit_message>
<xml_diff>
--- a/djpsilobus/assets/template.xlsx
+++ b/djpsilobus/assets/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
     <t>Course Number</t>
   </si>
   <si>
-    <t>Catelog Year</t>
+    <t>Catelog</t>
   </si>
   <si>
     <t>Year</t>
@@ -37,7 +37,7 @@
     <t>Section</t>
   </si>
   <si>
-    <t>Sub-Session</t>
+    <t>Sub-Section</t>
   </si>
   <si>
     <t>Course Title</t>
@@ -190,26 +190,26 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.03238866396761"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.39271255060729"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="57.7368421052632"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="8.81781376518219"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.0816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.6683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="5.89285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.89285714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.18877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3112244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="56.9030612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.1428571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="11.8979591836735"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.1428571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.5561224489796"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="16.9642857142857"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="8.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="10.3673469387755"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>